<commit_message>
Data Gather long 30mns
</commit_message>
<xml_diff>
--- a/django_thesis/Data_Gathering/VIVO Crowdsourcing Calibration Coefficients/cap1_2412_Realme_6Pro.xlsx
+++ b/django_thesis/Data_Gathering/VIVO Crowdsourcing Calibration Coefficients/cap1_2412_Realme_6Pro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thesis2.0\django_thesis\Data_Gathering\VIVO Crowdsourcing Calibration Coefficients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3B1C94-45E4-4CDD-9C24-FCBA15367C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6950FE7F-0F1A-4273-88DE-7EFAE7F6B000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1012,7 +1012,8 @@
         </a:gradFill>
         <a:ln>
           <a:solidFill>
-            <a:schemeClr val="tx1">
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
               <a:alpha val="95000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -2040,7 +2041,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>